<commit_message>
Añadir ideas.txt, notas.txt y cambios en Hardaware.xlsx
</commit_message>
<xml_diff>
--- a/Hardware.xlsx
+++ b/Hardware.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ariel\Documents\Skynet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9639ED27-6414-4475-8E50-C1102567D6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0917E802-477B-4FBC-A89C-82E9E10939C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Piezas</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Ruedas</t>
+  </si>
+  <si>
+    <t>Sensor Ultrasonico</t>
   </si>
 </sst>
 </file>
@@ -425,12 +428,12 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
     <col min="7" max="7" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -491,7 +494,9 @@
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="4"/>
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>

</xml_diff>

<commit_message>
Añadir archivo Notas Hardware.txt y Notas Software.txt
</commit_message>
<xml_diff>
--- a/Hardware.xlsx
+++ b/Hardware.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ariel\Documents\Skynet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0917E802-477B-4FBC-A89C-82E9E10939C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD585E1-24D6-483B-B832-21793FBDB79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>Link</t>
   </si>
   <si>
-    <t>Adicion</t>
-  </si>
-  <si>
     <t>Si</t>
   </si>
   <si>
@@ -65,6 +62,9 @@
   </si>
   <si>
     <t>Sensor Ultrasonico</t>
+  </si>
+  <si>
+    <t>Añadicion</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -451,18 +451,18 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -473,7 +473,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -484,7 +484,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -495,7 +495,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -585,12 +585,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios en Harware.xlsx e ideas.txt (precios y tareas)
</commit_message>
<xml_diff>
--- a/Hardware.xlsx
+++ b/Hardware.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ariel\Documents\Skynet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD585E1-24D6-483B-B832-21793FBDB79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5047E52-4200-43C2-977D-795D09D21CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,30 +16,32 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Piezas</t>
   </si>
   <si>
-    <t>Peso</t>
-  </si>
-  <si>
-    <t>Altura</t>
-  </si>
-  <si>
-    <t>Ancho</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
@@ -49,12 +51,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Arnuino</t>
-  </si>
-  <si>
-    <t>Precio</t>
-  </si>
-  <si>
     <t>Motor</t>
   </si>
   <si>
@@ -64,17 +60,86 @@
     <t>Sensor Ultrasonico</t>
   </si>
   <si>
-    <t>Añadicion</t>
+    <t>https://es.aliexpress.com/item/1005005467178145.html?spm=a2g0o.productlist.main.1.6cb01570FH2VZb&amp;algo_pvid=1defddeb-6547-43d1-a377-8cfd021645d3&amp;algo_exp_id=1defddeb-6547-43d1-a377-8cfd021645d3-0&amp;pdp_ext_f=%7B</t>
+  </si>
+  <si>
+    <t>Placa</t>
+  </si>
+  <si>
+    <t>https://es.aliexpress.com/item/1005008126137630.html?spm=a2g0o.detail.pcDetailTopMoreOtherSeller.3.72fa7928bgo95A&amp;gps-id=pcDetailTopMoreOtherSeller&amp;scm=1007.40196.366991.0&amp;scm_id=1007.40196.366991.0&amp;scm-url=1007.40196.366991.0&amp;pvid=1754c690-336c-4e36-b96b-1b71b517ef63&amp;_t=gps-id:pcDetailTopMoreOtherSeller,scm-url:1007.40196.366991.0,pvid:1754c690-336c-4e36-b96b-1b71b517ef63,tpp_buckets:668%232846%238111%231996&amp;pdp_ext_f=%7B%22order%22%3A%22141%22%2C%22eval%22%3A%221%22%2C%22sceneId%22%3A%2230050%22%7D&amp;pdp_npi=4%40dis%21MXN%2151.73%2141.68%21%21%2118.76%2115.12%21%402101c5a417451920026875027edec6%2112000043895581046%21rec%21MX%21%21ABX&amp;utparam-url=scene%3ApcDetailTopMoreOtherSeller%7Cquery_from%3A</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Vela</t>
+  </si>
+  <si>
+    <t>Arduino</t>
+  </si>
+  <si>
+    <t>Peso (g)</t>
+  </si>
+  <si>
+    <t>Altura (cm)</t>
+  </si>
+  <si>
+    <t>Ancho (cm)</t>
+  </si>
+  <si>
+    <t>Precio (MXN)</t>
+  </si>
+  <si>
+    <t>Añadicion (Si/No)</t>
+  </si>
+  <si>
+    <t>Bateria</t>
+  </si>
+  <si>
+    <t>Voltaje Min (V)</t>
+  </si>
+  <si>
+    <t>Voltaje Max (V)</t>
+  </si>
+  <si>
+    <t>https://es.aliexpress.com/item/1005002389227799.html?src=google&amp;pdp_npi=4%40dis!MXN!205.16!127.90!!!!!%40!12000020475407951!ppc!!!&amp;src=google&amp;albch=shopping&amp;acnt=742-864-1166&amp;isdl=y&amp;slnk=&amp;plac=&amp;mtctp=&amp;albbt=Google_7_shopping&amp;aff_platform=google&amp;aff_short_key=UneMJZVf&amp;gclsrc=aw.ds&amp;&amp;albagn=888888&amp;&amp;ds_e_adid=&amp;ds_e_matchtype=&amp;ds_e_device=c&amp;ds_e_network=x&amp;ds_e_product_group_id=&amp;ds_e_product_id=es1005002389227799&amp;ds_e_product_merchant_id=106603197&amp;ds_e_product_country=MX&amp;ds_e_product_language=es&amp;ds_e_product_channel=online&amp;ds_e_product_store_id=&amp;ds_url_v=2&amp;albcp=21989024792&amp;albag=&amp;isSmbAutoCall=false&amp;needSmbHouyi=false&amp;gad_source=1&amp;gbraid=0AAAAA99aYpdiUeyTg9XDYfoUCyp92APgU&amp;gclid=Cj0KCQjwtpLABhC7ARIsALBOCVr0Xqu3PjcQ720oKvSu6RGkW1MpILbKKi8qu2AQQ_qDcWSQXk2IRokaAl5FEALw_wcB</t>
+  </si>
+  <si>
+    <t>https://es.aliexpress.com/item/1005008613243786.html?spm=a2g0o.productlist.main.3.371enp3jnp3j9l&amp;algo_pvid=122afa11-d707-4f5f-a363-91c6c61b8e29&amp;algo_exp_id=122afa11-d707-4f5f-a363-91c6c61b8e29-2&amp;pdp_ext_f=%7B%22order%22%3A%2225%22%2C%22eval%22%3A%221%22%7D&amp;pdp_npi=4%40dis%21MXN%2162.69%2149.63%21%21%213.12%212.47%21%402103205117451998919314571ee129%2112000045951598938%21sea%21MX%210%21ABX&amp;curPageLogUid=8jR2FuPlBfmg&amp;utparam-url=scene%3Asearch%7Cquery_from%3A</t>
+  </si>
+  <si>
+    <t>Led infrarrojo</t>
+  </si>
+  <si>
+    <t>https://es.aliexpress.com/item/1005008464132772.html?spm=a2g0o.detail.pcDetailTopMoreOtherSeller.2.7ae2o70eo70eEa&amp;gps-id=pcDetailTopMoreOtherSeller&amp;scm=1007.40050.354490.0&amp;scm_id=1007.40050.354490.0&amp;scm-url=1007.40050.354490.0&amp;pvid=abe1c75b-d17a-4de7-a8c7-23104adb6cd4&amp;_t=gps-id:pcDetailTopMoreOtherSeller,scm-url:1007.40050.354490.0,pvid:abe1c75b-d17a-4de7-a8c7-23104adb6cd4,tpp_buckets:668%232846%238116%232002&amp;pdp_ext_f=%7B%22order%22%3A%2221%22%2C%22eval%22%3A%221%22%2C%22sceneId%22%3A%2230050%22%7D&amp;pdp_npi=4%40dis%21MXN%218.24%216.63%21%21%210.41%210.33%21%40210318c317452050442055393e6baa%2112000045244808419%21rec%21MX%21%21ABX&amp;utparam-url=scene%3ApcDetailTopMoreOtherSeller%7Cquery_from%3A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,17 +195,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,140 +507,270 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.453125" customWidth="1"/>
-    <col min="7" max="7" width="12.81640625" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" customWidth="1"/>
+    <col min="7" max="7" width="15.90625" customWidth="1"/>
+    <col min="9" max="9" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6">
+        <v>25</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6">
+        <v>6</v>
+      </c>
+      <c r="F2" s="6">
+        <v>20</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="4">
+        <v>35</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E3" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="F3" s="4">
+        <v>12</v>
+      </c>
+      <c r="G3" s="5">
+        <v>42</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1600</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G4" s="5">
+        <v>50</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <f>48*4</f>
+        <v>192</v>
+      </c>
+      <c r="C5" s="4">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="4"/>
+      <c r="G5" s="5">
+        <v>173</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
+      <c r="E6" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5</v>
+      </c>
+      <c r="G6" s="5">
+        <v>21</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G9" s="5">
+        <v>6</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G10" s="5"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4">
+        <f>SUM(B2:B11)/1000</f>
+        <v>1.8520000000000001</v>
+      </c>
+      <c r="C12" s="4">
+        <f>SUM(C2:C11)</f>
+        <v>5</v>
+      </c>
+      <c r="D12" s="4">
+        <f>SUM(D2:D11)</f>
+        <v>2</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" ref="E12:F12" si="0">SUM(E2:E11)</f>
+        <v>13.8</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="G12" s="5">
+        <f>SUM(G2:G11)</f>
+        <v>292</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H6" r:id="rId1" xr:uid="{A6E454A8-3FC0-4A68-B1EA-2C0ECCFE8080}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -567,7 +779,7 @@
           <x14:formula1>
             <xm:f>Hoja2!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>G2</xm:sqref>
+          <xm:sqref>I2:I12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -585,12 +797,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicion de tabla de precios con envios rapidos Hardware.xlsx
</commit_message>
<xml_diff>
--- a/Hardware.xlsx
+++ b/Hardware.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ariel\Documents\Skynet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5047E52-4200-43C2-977D-795D09D21CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019D5A70-A6B3-4101-95A4-DC8E8F9FD45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
   <si>
     <t>Piezas</t>
   </si>
@@ -51,9 +51,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Motor</t>
-  </si>
-  <si>
     <t>Ruedas</t>
   </si>
   <si>
@@ -112,6 +109,42 @@
   </si>
   <si>
     <t>https://es.aliexpress.com/item/1005008464132772.html?spm=a2g0o.detail.pcDetailTopMoreOtherSeller.2.7ae2o70eo70eEa&amp;gps-id=pcDetailTopMoreOtherSeller&amp;scm=1007.40050.354490.0&amp;scm_id=1007.40050.354490.0&amp;scm-url=1007.40050.354490.0&amp;pvid=abe1c75b-d17a-4de7-a8c7-23104adb6cd4&amp;_t=gps-id:pcDetailTopMoreOtherSeller,scm-url:1007.40050.354490.0,pvid:abe1c75b-d17a-4de7-a8c7-23104adb6cd4,tpp_buckets:668%232846%238116%232002&amp;pdp_ext_f=%7B%22order%22%3A%2221%22%2C%22eval%22%3A%221%22%2C%22sceneId%22%3A%2230050%22%7D&amp;pdp_npi=4%40dis%21MXN%218.24%216.63%21%21%210.41%210.33%21%40210318c317452050442055393e6baa%2112000045244808419%21rec%21MX%21%21ABX&amp;utparam-url=scene%3ApcDetailTopMoreOtherSeller%7Cquery_from%3A</t>
+  </si>
+  <si>
+    <t>Servomotor</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Oruga</t>
+  </si>
+  <si>
+    <t>Sensor Infrrojo</t>
+  </si>
+  <si>
+    <t>Precio (c/d) (MXM)</t>
+  </si>
+  <si>
+    <t>https://articulo.mercadolibre.com.mx/MLM-1346794889-4-piezas-mg90s-servomotor-engranes-metalicos-arduino-_JM#polycard_client=search-nordic&amp;position=5&amp;search_layout=stack&amp;type=item&amp;tracking_id=e85be694-a5b8-4bc0-bd3f-ec15974006da&amp;wid=MLM1346794889&amp;sid=search</t>
+  </si>
+  <si>
+    <t>Servomotor Mg90s</t>
+  </si>
+  <si>
+    <t>https://www.mercadolibre.com.mx/2-juegos-de-oruga-rueda-motriz-rueda-de-oruga-y-rueda-de-r/p/MLM2012814151#polycard_client=search-nordic&amp;searchVariation=MLM2012814151&amp;wid=MLM3537810278&amp;position=27&amp;search_layout=grid&amp;type=product&amp;tracking_id=e73711f8-be14-4d9b-a32c-2b97c3f1bf45&amp;sid=search</t>
+  </si>
+  <si>
+    <t>Sensor Ultrasonico Hc-sr04</t>
+  </si>
+  <si>
+    <t>https://articulo.mercadolibre.com.mx/MLM-603602115-sensor-ultrasonico-hc-sr04-_JM#polycard_client=search-nordic&amp;position=22&amp;search_layout=stack&amp;type=item&amp;tracking_id=039cca01-70ad-45ea-a9ee-879ce6e1f3af&amp;wid=MLM603602115&amp;sid=search</t>
+  </si>
+  <si>
+    <t>https://articulo.mercadolibre.com.mx/MLM-550268351-modulo-sensor-de-obstaculos-reflectivo-infrarojo-arduino-_JM#polycard_client=search-nordic&amp;position=24&amp;search_layout=stack&amp;type=item&amp;tracking_id=a837bd40-715d-4f60-a129-51d3470342af&amp;wid=MLM550268351&amp;sid=search</t>
+  </si>
+  <si>
+    <t>https://articulo.mercadolibre.com.mx/MLM-2942137662-led-infrarrojo-y-fotodiodo-emisor-receptor-5-pares-_JM?searchVariation=180054798536#polycard_client=search-nordic&amp;searchVariation=180054798536&amp;position=14&amp;search_layout=stack&amp;type=item&amp;tracking_id=e2928182-0370-4b6a-a2f0-6843e29d4927</t>
   </si>
 </sst>
 </file>
@@ -213,12 +246,12 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -507,76 +540,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" customWidth="1"/>
     <col min="3" max="3" width="11.1796875" customWidth="1"/>
     <col min="4" max="4" width="12.54296875" customWidth="1"/>
     <col min="5" max="5" width="16.08984375" customWidth="1"/>
     <col min="6" max="6" width="16.36328125" customWidth="1"/>
     <col min="7" max="7" width="15.90625" customWidth="1"/>
-    <col min="9" max="9" width="16.81640625" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" customWidth="1"/>
+    <col min="10" max="10" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4">
         <v>25</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4">
         <v>6</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="4">
         <v>20</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="6"/>
       <c r="I2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4">
         <v>35</v>
@@ -592,16 +626,16 @@
       <c r="G3" s="5">
         <v>42</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>9</v>
+      <c r="H3" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B4" s="4">
         <v>1600</v>
@@ -613,16 +647,16 @@
       <c r="G4" s="5">
         <v>50</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>22</v>
+      <c r="H4" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4">
         <f>48*4</f>
@@ -639,16 +673,16 @@
       <c r="G5" s="5">
         <v>173</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>21</v>
+      <c r="H5" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -662,16 +696,16 @@
       <c r="G6" s="5">
         <v>21</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>7</v>
+      <c r="H6" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -679,12 +713,12 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="8"/>
+      <c r="H7" s="6"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -692,12 +726,12 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="8"/>
+      <c r="H8" s="6"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -707,14 +741,14 @@
       <c r="G9" s="5">
         <v>6</v>
       </c>
-      <c r="H9" s="8" t="s">
-        <v>24</v>
+      <c r="H9" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -722,10 +756,10 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="8"/>
+      <c r="H10" s="6"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -733,12 +767,12 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="8"/>
+      <c r="H11" s="6"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4">
         <f>SUM(B2:B11)/1000</f>
@@ -767,9 +801,289 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="4">
+        <v>25</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1600</v>
+      </c>
+      <c r="C16" s="4">
+        <v>4</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4">
+        <v>190</v>
+      </c>
+      <c r="I16" s="6">
+        <v>190</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="4">
+        <f>48*4</f>
+        <v>192</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4">
+        <v>445</v>
+      </c>
+      <c r="I17" s="6">
+        <v>445</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="G18" s="4">
+        <v>5</v>
+      </c>
+      <c r="H18" s="4">
+        <v>55</v>
+      </c>
+      <c r="I18" s="9">
+        <v>55</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4">
+        <v>42</v>
+      </c>
+      <c r="I19" s="6">
+        <v>42</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4">
+        <v>52</v>
+      </c>
+      <c r="I22" s="6">
+        <v>52</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="4">
+        <f>SUM(B15:B24)/1000</f>
+        <v>1.8169999999999999</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4">
+        <f>SUM(D15:D24)</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="4">
+        <f>SUM(E15:E24)</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
+        <f>SUM(F15:F24)</f>
+        <v>3.3</v>
+      </c>
+      <c r="G25" s="4">
+        <f>SUM(G15:G24)</f>
+        <v>5</v>
+      </c>
+      <c r="H25" s="4"/>
+      <c r="I25" s="5">
+        <f>SUM(I15:I24)</f>
+        <v>784</v>
+      </c>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H6" r:id="rId1" xr:uid="{A6E454A8-3FC0-4A68-B1EA-2C0ECCFE8080}"/>
+    <hyperlink ref="J18" r:id="rId2" location="polycard_client=search-nordic&amp;position=22&amp;search_layout=stack&amp;type=item&amp;tracking_id=039cca01-70ad-45ea-a9ee-879ce6e1f3af&amp;wid=MLM603602115&amp;sid=search" xr:uid="{F45A2B47-039C-4443-8483-1F0987A7391F}"/>
+    <hyperlink ref="J16" r:id="rId3" location="polycard_client=search-nordic&amp;position=5&amp;search_layout=stack&amp;type=item&amp;tracking_id=e85be694-a5b8-4bc0-bd3f-ec15974006da&amp;wid=MLM1346794889&amp;sid=search" display="https://articulo.mercadolibre.com.mx/MLM-1346794889-4-piezas-mg90s-servomotor-engranes-metalicos-arduino-_JM#polycard_client=search-nordic&amp;position=5&amp;search_layout=stack&amp;type=item&amp;tracking_id=e85be694-a5b8-4bc0-bd3f-ec15974006da&amp;wid=MLM1346794889&amp;sid=search" xr:uid="{68542A16-C504-471D-B60C-7A569DE6B8F6}"/>
+    <hyperlink ref="J17" r:id="rId4" location="polycard_client=search-nordic&amp;searchVariation=MLM2012814151&amp;wid=MLM3537810278&amp;position=27&amp;search_layout=grid&amp;type=product&amp;tracking_id=e73711f8-be14-4d9b-a32c-2b97c3f1bf45&amp;sid=search" display="https://www.mercadolibre.com.mx/2-juegos-de-oruga-rueda-motriz-rueda-de-oruga-y-rueda-de-r/p/MLM2012814151#polycard_client=search-nordic&amp;searchVariation=MLM2012814151&amp;wid=MLM3537810278&amp;position=27&amp;search_layout=grid&amp;type=product&amp;tracking_id=e73711f8-be14-4d9b-a32c-2b97c3f1bf45&amp;sid=search" xr:uid="{133E5518-F1A3-4B59-88ED-4EDA2E0B5F34}"/>
+    <hyperlink ref="J19" r:id="rId5" location="polycard_client=search-nordic&amp;position=24&amp;search_layout=stack&amp;type=item&amp;tracking_id=a837bd40-715d-4f60-a129-51d3470342af&amp;wid=MLM550268351&amp;sid=search" display="https://articulo.mercadolibre.com.mx/MLM-550268351-modulo-sensor-de-obstaculos-reflectivo-infrarojo-arduino-_JM#polycard_client=search-nordic&amp;position=24&amp;search_layout=stack&amp;type=item&amp;tracking_id=a837bd40-715d-4f60-a129-51d3470342af&amp;wid=MLM550268351&amp;sid=search" xr:uid="{D73A7DA8-19A9-4A15-A7D4-BD792DE06A4A}"/>
+    <hyperlink ref="J22" r:id="rId6" location="polycard_client=search-nordic&amp;searchVariation=180054798536&amp;position=14&amp;search_layout=stack&amp;type=item&amp;tracking_id=e2928182-0370-4b6a-a2f0-6843e29d4927" display="https://articulo.mercadolibre.com.mx/MLM-2942137662-led-infrarrojo-y-fotodiodo-emisor-receptor-5-pares-_JM?searchVariation=180054798536#polycard_client=search-nordic&amp;searchVariation=180054798536&amp;position=14&amp;search_layout=stack&amp;type=item&amp;tracking_id=e2928182-0370-4b6a-a2f0-6843e29d4927" xr:uid="{78F3912B-5F22-428A-B610-0DE3EEFABCA1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -779,7 +1093,7 @@
           <x14:formula1>
             <xm:f>Hoja2!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I12</xm:sqref>
+          <xm:sqref>I2:I12 K15:K25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>